<commit_message>
sprints aktualisiert und Class Diagramm hochgeladen
</commit_message>
<xml_diff>
--- a/doc/CS1task10/scrum_task10_EN.xlsx
+++ b/doc/CS1task10/scrum_task10_EN.xlsx
@@ -1,31 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gian-Andrea/Dropbox (Degen's HD)/medizininformatik/5. semester/software engineering and design/case studies/software_e_white/Summaries_Tasks/CS1/CS1 Task10/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="15060" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="5" r:id="rId2"/>
-    <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint Backlog" sheetId="7" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product Backlog'!$A$1:$M$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$A$1:$L$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$A$1:$L$38</definedName>
   </definedNames>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -216,9 +208,6 @@
     <t>Total h</t>
   </si>
   <si>
-    <t xml:space="preserve">Documents are sent by mail/e-mail. Documents will be filed in </t>
-  </si>
-  <si>
     <t>Sprint</t>
   </si>
   <si>
@@ -231,15 +220,6 @@
     <t>Reviewer</t>
   </si>
   <si>
-    <t>Base frame</t>
-  </si>
-  <si>
-    <t>Create packages/main classes</t>
-  </si>
-  <si>
-    <t>Software architecture</t>
-  </si>
-  <si>
     <t>Fabienne</t>
   </si>
   <si>
@@ -355,6 +335,108 @@
   </si>
   <si>
     <t>Remaining Ressources</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Client Class</t>
+  </si>
+  <si>
+    <t>waiting</t>
+  </si>
+  <si>
+    <t>stopped</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>Database class</t>
+  </si>
+  <si>
+    <t>Address Class</t>
+  </si>
+  <si>
+    <t>Caregiver Class</t>
+  </si>
+  <si>
+    <t>Contact Class</t>
+  </si>
+  <si>
+    <t>ExternalInstitution Class</t>
+  </si>
+  <si>
+    <t>Person Class</t>
+  </si>
+  <si>
+    <t>Communication Class</t>
+  </si>
+  <si>
+    <t>ExternalPerson Class</t>
+  </si>
+  <si>
+    <t>Gian</t>
+  </si>
+  <si>
+    <t>Network Class</t>
+  </si>
+  <si>
+    <t>Implementing GUI, multiple Views</t>
+  </si>
+  <si>
+    <t>Implementing logic for Database connection</t>
+  </si>
+  <si>
+    <t>Implementing logic for CRUD</t>
+  </si>
+  <si>
+    <t>Creating Connection between program and database</t>
+  </si>
+  <si>
+    <t>Activity Reporting class</t>
+  </si>
+  <si>
+    <t>Bill class</t>
+  </si>
+  <si>
+    <t>Calender class</t>
+  </si>
+  <si>
+    <t>Meddoku class</t>
+  </si>
+  <si>
+    <t>Statistics class</t>
+  </si>
+  <si>
+    <t>All Classes</t>
+  </si>
+  <si>
+    <t>Changing structure</t>
+  </si>
+  <si>
+    <t>Model, View, data base</t>
+  </si>
+  <si>
+    <t>Total h Sprint 1</t>
+  </si>
+  <si>
+    <t>Total h Sprint 2</t>
+  </si>
+  <si>
+    <t>Total h Sprint 3</t>
+  </si>
+  <si>
+    <t>Adapting GUI for smartphone</t>
+  </si>
+  <si>
+    <t>Optimse Code</t>
+  </si>
+  <si>
+    <t>for all classes</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -443,12 +525,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -498,11 +608,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="31">
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -515,6 +663,610 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.73344444444444434"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>BurndownChart!$A$2:$B$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="3"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>02.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>08.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>09.12.2016</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Ressources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>BurndownChart!$A$2:$B$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="3"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>02.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>08.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>09.12.2016</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="107245568"/>
+        <c:axId val="107247104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="107245568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107247104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="107247104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107245568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.71808906052348553"/>
+          <c:y val="3.8585209003215437E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.2182852143482065E-2"/>
+          <c:y val="7.4548702245552642E-2"/>
+          <c:w val="0.53169094488188973"/>
+          <c:h val="0.59207932341790614"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>BurndownChart!$A$22:$B$26</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>09.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>15.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>22.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>23.12.2016</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$C$22:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Ressources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>BurndownChart!$A$22:$B$26</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>09.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>15.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>22.12.2016</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>23.12.2016</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$22:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="220443008"/>
+        <c:axId val="220444544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="220443008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="220444544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="220444544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="220443008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,13 +1562,13 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -824,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -832,7 +1584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -840,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -848,7 +1600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -856,7 +1608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -864,7 +1616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -872,7 +1624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -882,29 +1634,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -930,7 +1687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -948,7 +1705,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -966,7 +1723,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -984,7 +1741,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1002,7 +1759,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1018,7 +1775,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1034,7 +1791,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1052,7 +1809,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1068,7 +1825,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1084,7 +1841,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1100,7 +1857,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1116,7 +1873,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1134,7 +1891,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1152,7 +1909,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1170,7 +1927,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1188,7 +1945,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1204,7 +1961,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="13" t="s">
         <v>59</v>
       </c>
@@ -1213,48 +1970,49 @@
         <v>221.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-    </row>
+    <row r="20" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:M17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="125" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1263,13 +2021,13 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>19</v>
@@ -1287,589 +2045,1981 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="1">
+        <v>10</v>
+      </c>
+      <c r="K5" s="1">
+        <v>10</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="18" t="s">
-        <v>83</v>
+      <c r="F6" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1">
+        <v>6</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I9" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>1.9</v>
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>1.1000000000000001</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I11" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>1.1100000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>2</v>
       </c>
       <c r="B13" s="7">
         <v>1</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="B14" s="7">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I14" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="B15" s="7">
         <v>1</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="D15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="I15" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15">
-        <v>4.0999999999999996</v>
+        <v>2.5</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>13</v>
       </c>
       <c r="B17" s="7">
         <v>1</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>70</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I17" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>13.1</v>
       </c>
       <c r="B18" s="7">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>74</v>
+        <v>95</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I18" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="15">
-        <v>13.1</v>
-      </c>
-      <c r="B19" s="7">
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B19" s="20">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="2">
+        <v>6</v>
+      </c>
+      <c r="J19" s="2">
+        <v>20</v>
+      </c>
+      <c r="K19" s="2">
+        <v>15</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B20" s="20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="2">
+        <v>6</v>
+      </c>
+      <c r="J20" s="2">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2">
+        <v>15</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B21" s="20">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="2">
+        <v>6</v>
+      </c>
+      <c r="J21" s="2">
+        <v>10</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B22" s="20">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="2">
+        <v>4</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2">
+        <v>8</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <v>16</v>
+      </c>
+      <c r="B23" s="20">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="2">
+        <v>3</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2">
+        <v>5</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B24" s="20">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2">
+        <v>7</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <v>13.2</v>
+      </c>
+      <c r="B25" s="20">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2">
+        <v>5</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>13.3</v>
+      </c>
+      <c r="B26" s="20">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2">
+        <v>6</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="B27" s="20">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2">
+        <v>5</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <v>13.4</v>
+      </c>
+      <c r="B28" s="20">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
+        <v>1.18</v>
+      </c>
+      <c r="B29" s="20">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="2">
+        <v>6</v>
+      </c>
+      <c r="J29" s="2">
+        <v>12</v>
+      </c>
+      <c r="K29" s="2">
+        <v>12</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <v>13.5</v>
+      </c>
+      <c r="B30" s="20">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="2">
+        <v>8</v>
+      </c>
+      <c r="J30" s="2">
+        <v>12</v>
+      </c>
+      <c r="K30" s="2">
+        <v>12</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B31" s="20">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="2">
+        <v>6</v>
+      </c>
+      <c r="J31" s="2">
+        <v>10</v>
+      </c>
+      <c r="K31" s="2">
+        <v>10</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <v>8</v>
+      </c>
+      <c r="B32" s="20">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="2">
+        <v>4</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21">
+        <v>4.2</v>
+      </c>
+      <c r="B33" s="20">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="2">
+        <v>4</v>
+      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21">
+        <v>9</v>
+      </c>
+      <c r="B34" s="20">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="2">
+        <v>4</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21">
+        <v>15</v>
+      </c>
+      <c r="B35" s="20">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="2">
+        <v>6</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21">
+        <v>10</v>
+      </c>
+      <c r="B36" s="20">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="2">
+        <v>6</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21">
+        <v>7</v>
+      </c>
+      <c r="B37" s="20">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19">
+        <v>1.19</v>
+      </c>
+      <c r="B38" s="20">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="2">
+        <v>6</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2">
+        <v>6</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="B39" s="7">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" s="1">
+        <v>4</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="B40" s="7">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="1">
+        <v>4</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="B41" s="7">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="1">
+        <v>4</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B42" s="7">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I42" s="1">
+        <v>4</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B43" s="7">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43" s="1">
+        <v>4</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="19">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B44" s="20">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I44" s="2">
+        <v>10</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="19">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B45" s="20">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" s="2">
+        <v>6</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B46" s="20">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I46" s="2">
+        <v>6</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B47" s="7">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" s="1">
+        <v>10</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <v>13</v>
+      </c>
+      <c r="B48" s="7">
+        <v>3</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" s="1">
+        <v>8</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
         <v>1</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="B49" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="8"/>
-      <c r="H21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="13">
-        <f>SUM(I2:I19)</f>
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G25" s="1"/>
-    </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-    </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-    </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-    </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-    </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
+      <c r="C49" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" s="1">
+        <v>10</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D53" s="8"/>
+      <c r="H53" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I53" s="22">
+        <f>SUM(I2:I18)</f>
+        <v>42</v>
+      </c>
+      <c r="K53" s="22">
+        <f>SUM(K2:K18)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D54" s="8"/>
+      <c r="H54" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I54" s="22">
+        <f>SUM(I19:I38)</f>
+        <v>98</v>
+      </c>
+      <c r="K54" s="22">
+        <f>SUM(K20:K38)</f>
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G55" s="1"/>
+      <c r="H55" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="I55" s="22">
+        <f>SUM(I39:I49)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L19"/>
+  <autoFilter ref="A1:L38"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="6"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>42706</v>
+      </c>
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42712</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>42713</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6">
+        <v>42713</v>
+      </c>
+      <c r="C22">
+        <v>98</v>
+      </c>
+      <c r="D22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="6">
+        <v>42719</v>
+      </c>
+      <c r="C23">
+        <v>93</v>
+      </c>
+      <c r="D23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6">
+        <v>42720</v>
+      </c>
+      <c r="C24">
+        <v>92</v>
+      </c>
+      <c r="D24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6">
+        <v>42726</v>
+      </c>
+      <c r="C25">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="6">
+        <v>42727</v>
+      </c>
+      <c r="C26">
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42" s="6">
+        <v>42727</v>
+      </c>
+      <c r="C42">
+        <v>70</v>
+      </c>
+      <c r="D42">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>